<commit_message>
Alteração da tabela e diagrama de casos de uso
</commit_message>
<xml_diff>
--- a/tabela de casos de uso.xlsx
+++ b/tabela de casos de uso.xlsx
@@ -27,9 +27,6 @@
     <t>Objetivos</t>
   </si>
   <si>
-    <t>Diretor</t>
-  </si>
-  <si>
     <t>Rececionista</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>O objetivo é Configurar as condições do Wather API</t>
+  </si>
+  <si>
+    <t>Diretor do Hotel</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C19"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,54 +521,54 @@
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" ref="B7:C9" si="0">B4</f>
@@ -604,97 +604,97 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizei tabela de casos de uso e relatório
Indices já funcionem
</commit_message>
<xml_diff>
--- a/tabela de casos de uso.xlsx
+++ b/tabela de casos de uso.xlsx
@@ -498,14 +498,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:A10"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="A1:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adicionei o caso de uso "eliminar promoção"
não completo
</commit_message>
<xml_diff>
--- a/tabela de casos de uso.xlsx
+++ b/tabela de casos de uso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Ator</t>
   </si>
@@ -117,9 +117,6 @@
     <t>O objetivo é receber as possíveis promoções para depois segmentar ou recusar</t>
   </si>
   <si>
-    <t>O objetivo é torna-las ativas</t>
-  </si>
-  <si>
     <t>O objetivo é registar uma promoção</t>
   </si>
   <si>
@@ -130,6 +127,15 @@
   </si>
   <si>
     <t>Diretor do Hotel</t>
+  </si>
+  <si>
+    <t>Eliminar Promoção</t>
+  </si>
+  <si>
+    <t>O objetivo é torna-la inativa</t>
+  </si>
+  <si>
+    <t>O objetivo é torna-la ativa</t>
   </si>
 </sst>
 </file>
@@ -180,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -193,6 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,11 +501,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="A1:C19"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +528,7 @@
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -649,7 +656,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -676,7 +683,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -691,17 +698,26 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>36</v>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A13:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>